<commit_message>
Add download photos in Excel
</commit_message>
<xml_diff>
--- a/templates/報名表.xlsx
+++ b/templates/報名表.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljchen/Desktop/Study/sport/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D34C83-CBBE-2244-9227-A57FA40166B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE72181C-8400-F04E-983E-441A69421F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="11420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="報名表資料" sheetId="1" r:id="rId1"/>
+    <sheet name="報名表照片" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>背號</t>
   </si>
@@ -66,6 +67,93 @@
   </si>
   <si>
     <t>隊長：</t>
+  </si>
+  <si>
+    <t>附件二：報名表照片</t>
+  </si>
+  <si>
+    <t>1.姓名：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.姓名：</t>
+  </si>
+  <si>
+    <t>3.姓名：</t>
+  </si>
+  <si>
+    <t>4.姓名：</t>
+  </si>
+  <si>
+    <t>5.姓名：</t>
+  </si>
+  <si>
+    <t>6.姓名：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.姓名：</t>
+  </si>
+  <si>
+    <t>8.姓名：</t>
+  </si>
+  <si>
+    <t>9.姓名：</t>
+  </si>
+  <si>
+    <t>10.姓名：</t>
+  </si>
+  <si>
+    <t>11.姓名：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.姓名：</t>
+  </si>
+  <si>
+    <t>13.姓名：</t>
+  </si>
+  <si>
+    <t>14.姓名：</t>
+  </si>
+  <si>
+    <t>15.姓名：</t>
+  </si>
+  <si>
+    <t>16.姓名：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17.姓名：</t>
+  </si>
+  <si>
+    <t>18.姓名：</t>
+  </si>
+  <si>
+    <t>19.姓名：</t>
+  </si>
+  <si>
+    <t>20.姓名：</t>
+  </si>
+  <si>
+    <t>21.姓名：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22.姓名：</t>
+  </si>
+  <si>
+    <t>23.姓名：</t>
+  </si>
+  <si>
+    <t>24.姓名：</t>
+  </si>
+  <si>
+    <t>25.姓名：</t>
+  </si>
+  <si>
+    <t>序號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -75,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +189,26 @@
       <sz val="14"/>
       <name val="KaiTi"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="BiauKai"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="KaiTi"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,6 +268,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,7 +592,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -524,7 +650,9 @@
       <c r="G5" s="7"/>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1" ht="22" customHeight="1">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
@@ -828,4 +956,194 @@
 蓋 章</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F800AAF-5297-4E4E-9FA8-D9DC9261DBEE}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="5" width="19.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17">
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="17">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="23" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="17" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="91" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="15">
+      <c r="A7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="91" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" s="12" customFormat="1" ht="15">
+      <c r="A9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="91" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="15">
+      <c r="A11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="91" customHeight="1">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" s="12" customFormat="1" ht="15">
+      <c r="A13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="91" customHeight="1">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" s="12" customFormat="1" ht="15">
+      <c r="A15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update template.xlsx and .env
</commit_message>
<xml_diff>
--- a/templates/報名表.xlsx
+++ b/templates/報名表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morris/Desktop/sport/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7E83B2-97AD-2844-983E-55800F152C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAF207F-9463-2B48-9279-01A0D4254AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.45" right="0.45" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.2" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"楷體-簡 標準體,標準"＊本資料僅提供賽事資格證明&amp;C&amp;"楷體-簡 標準體,標準"系 所

</xml_diff>

<commit_message>
Fix 報名表.xlsx save pdf
</commit_message>
<xml_diff>
--- a/templates/報名表.xlsx
+++ b/templates/報名表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/morris/Desktop/sport/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAF207F-9463-2B48-9279-01A0D4254AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5703137-5BC7-AE4B-9C57-5D97CCCDFA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1003,7 +1003,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.2" right="0.2" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"楷體-簡 標準體,標準"＊本資料僅提供賽事資格證明&amp;C&amp;"楷體-簡 標準體,標準"系 所

</xml_diff>